<commit_message>
Added pull down resisotors to NAND gates. Maybe 'single' will be button.
</commit_message>
<xml_diff>
--- a/IC.xlsx
+++ b/IC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB20252-8E1E-4CD6-BAC0-016E3EB127ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FFA57-4ECD-41B6-ADDF-45F744B5EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>RAM</t>
   </si>
@@ -67,18 +67,6 @@
     <t>CLOCK</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>PINS-2*x-M</t>
   </si>
   <si>
@@ -128,16 +116,211 @@
   </si>
   <si>
     <t>2*1</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V9</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V13</t>
+  </si>
+  <si>
+    <t>V14</t>
+  </si>
+  <si>
+    <t>V15</t>
+  </si>
+  <si>
+    <t>V16</t>
+  </si>
+  <si>
+    <t>V17</t>
+  </si>
+  <si>
+    <t>V18</t>
+  </si>
+  <si>
+    <t>V19</t>
+  </si>
+  <si>
+    <t>V20</t>
+  </si>
+  <si>
+    <t>V21</t>
+  </si>
+  <si>
+    <t>V22</t>
+  </si>
+  <si>
+    <t>V23</t>
+  </si>
+  <si>
+    <t>V24</t>
+  </si>
+  <si>
+    <t>V25</t>
+  </si>
+  <si>
+    <t>V26</t>
+  </si>
+  <si>
+    <t>V27</t>
+  </si>
+  <si>
+    <t>V28</t>
+  </si>
+  <si>
+    <t>V29</t>
+  </si>
+  <si>
+    <t>V30</t>
+  </si>
+  <si>
+    <t>V31</t>
+  </si>
+  <si>
+    <t>V32</t>
+  </si>
+  <si>
+    <t>V33</t>
+  </si>
+  <si>
+    <t>V34</t>
+  </si>
+  <si>
+    <t>V35</t>
+  </si>
+  <si>
+    <t>V36</t>
+  </si>
+  <si>
+    <t>V37</t>
+  </si>
+  <si>
+    <t>V38</t>
+  </si>
+  <si>
+    <t>V39</t>
+  </si>
+  <si>
+    <t>V40</t>
+  </si>
+  <si>
+    <t>V41</t>
+  </si>
+  <si>
+    <t>V42</t>
+  </si>
+  <si>
+    <t>V43</t>
+  </si>
+  <si>
+    <t>V44</t>
+  </si>
+  <si>
+    <t>V45</t>
+  </si>
+  <si>
+    <t>V46</t>
+  </si>
+  <si>
+    <t>V47</t>
+  </si>
+  <si>
+    <t>V48</t>
+  </si>
+  <si>
+    <t>V49</t>
+  </si>
+  <si>
+    <t>V50</t>
+  </si>
+  <si>
+    <t>V51</t>
+  </si>
+  <si>
+    <t>V52</t>
+  </si>
+  <si>
+    <t>V53</t>
+  </si>
+  <si>
+    <t>V54</t>
+  </si>
+  <si>
+    <t>V55</t>
+  </si>
+  <si>
+    <t>V56</t>
+  </si>
+  <si>
+    <t>V57</t>
+  </si>
+  <si>
+    <t>V58</t>
+  </si>
+  <si>
+    <t>V59</t>
+  </si>
+  <si>
+    <t>V60</t>
+  </si>
+  <si>
+    <t>V61</t>
+  </si>
+  <si>
+    <t>V62</t>
+  </si>
+  <si>
+    <t>V63</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,10 +650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,34 +669,34 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
         <v>0</v>
@@ -528,10 +711,10 @@
         <v>5</v>
       </c>
       <c r="R1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -539,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <f>SUM(C2:S2)</f>
+        <f t="shared" ref="B2:B23" si="0">SUM(C2:S2)</f>
         <v>502</v>
       </c>
       <c r="C2">
@@ -611,7 +794,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <f>SUM(C3:S3)</f>
+        <f t="shared" si="0"/>
         <v>322</v>
       </c>
       <c r="C3" s="1"/>
@@ -646,19 +829,19 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <f>SUM(C4:S4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -666,11 +849,11 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -680,10 +863,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <f>SUM(C5:S5)</f>
+        <f t="shared" si="0"/>
         <v>235</v>
       </c>
       <c r="C5">
@@ -728,10 +911,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <f>SUM(C6:S6)</f>
+        <f t="shared" si="0"/>
         <v>235</v>
       </c>
       <c r="C6">
@@ -780,7 +963,7 @@
         <v>555</v>
       </c>
       <c r="B7">
-        <f>SUM(C7:S7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="1"/>
@@ -808,7 +991,7 @@
         <v>7400</v>
       </c>
       <c r="B8">
-        <f>SUM(C8:S8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C8" s="1"/>
@@ -838,7 +1021,7 @@
         <v>7402</v>
       </c>
       <c r="B9">
-        <f>SUM(C9:S9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="1"/>
@@ -866,7 +1049,7 @@
         <v>7404</v>
       </c>
       <c r="B10">
-        <f>SUM(C10:S10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C10" s="1"/>
@@ -894,7 +1077,7 @@
         <v>7408</v>
       </c>
       <c r="B11">
-        <f>SUM(C11:S11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C11" s="1"/>
@@ -924,7 +1107,7 @@
         <v>7410</v>
       </c>
       <c r="B12">
-        <f>SUM(C12:S12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="1"/>
@@ -952,7 +1135,7 @@
         <v>7432</v>
       </c>
       <c r="B13">
-        <f>SUM(C13:S13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C13" s="1"/>
@@ -978,7 +1161,7 @@
         <v>7430</v>
       </c>
       <c r="B14">
-        <f>SUM(C14:S14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C14" s="1"/>
@@ -1004,7 +1187,7 @@
         <v>7485</v>
       </c>
       <c r="B15">
-        <f>SUM(C15:S15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C15" s="1"/>
@@ -1032,7 +1215,7 @@
         <v>7486</v>
       </c>
       <c r="B16">
-        <f>SUM(C16:S16)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C16" s="1"/>
@@ -1060,7 +1243,7 @@
         <v>74112</v>
       </c>
       <c r="B17">
-        <f>SUM(C17:S17)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C17" s="1"/>
@@ -1088,7 +1271,7 @@
         <v>74138</v>
       </c>
       <c r="B18">
-        <f>SUM(C18:S18)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C18" s="1"/>
@@ -1118,7 +1301,7 @@
         <v>74193</v>
       </c>
       <c r="B19">
-        <f>SUM(C19:S19)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C19" s="1"/>
@@ -1146,7 +1329,7 @@
         <v>74245</v>
       </c>
       <c r="B20">
-        <f>SUM(C20:S20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C20">
@@ -1190,7 +1373,7 @@
         <v>74273</v>
       </c>
       <c r="B21">
-        <f>SUM(C21:S21)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21">
@@ -1232,7 +1415,7 @@
         <v>74283</v>
       </c>
       <c r="B22">
-        <f>SUM(C22:S22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C22" s="1"/>
@@ -1260,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <f>SUM(C23:S23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C23" s="1"/>
@@ -1285,10 +1468,344 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>7411</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>7404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>7408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:A21">
     <sortCondition ref="A7:A21"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
IC list for ctrl.
</commit_message>
<xml_diff>
--- a/IC.xlsx
+++ b/IC.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FFA57-4ECD-41B6-ADDF-45F744B5EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6917CC24-2E15-4533-9E32-9042E6AFD5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>RAM</t>
   </si>
@@ -196,115 +195,19 @@
     <t>V26</t>
   </si>
   <si>
-    <t>V27</t>
-  </si>
-  <si>
-    <t>V28</t>
-  </si>
-  <si>
-    <t>V29</t>
-  </si>
-  <si>
-    <t>V30</t>
-  </si>
-  <si>
-    <t>V31</t>
-  </si>
-  <si>
-    <t>V32</t>
-  </si>
-  <si>
-    <t>V33</t>
-  </si>
-  <si>
-    <t>V34</t>
-  </si>
-  <si>
-    <t>V35</t>
-  </si>
-  <si>
-    <t>V36</t>
-  </si>
-  <si>
-    <t>V37</t>
-  </si>
-  <si>
-    <t>V38</t>
-  </si>
-  <si>
-    <t>V39</t>
-  </si>
-  <si>
-    <t>V40</t>
-  </si>
-  <si>
-    <t>V41</t>
-  </si>
-  <si>
-    <t>V42</t>
-  </si>
-  <si>
-    <t>V43</t>
-  </si>
-  <si>
-    <t>V44</t>
-  </si>
-  <si>
-    <t>V45</t>
-  </si>
-  <si>
-    <t>V46</t>
-  </si>
-  <si>
-    <t>V47</t>
-  </si>
-  <si>
-    <t>V48</t>
-  </si>
-  <si>
-    <t>V49</t>
-  </si>
-  <si>
-    <t>V50</t>
-  </si>
-  <si>
-    <t>V51</t>
-  </si>
-  <si>
-    <t>V52</t>
-  </si>
-  <si>
-    <t>V53</t>
-  </si>
-  <si>
-    <t>V54</t>
-  </si>
-  <si>
-    <t>V55</t>
-  </si>
-  <si>
-    <t>V56</t>
-  </si>
-  <si>
-    <t>V57</t>
-  </si>
-  <si>
-    <t>V58</t>
-  </si>
-  <si>
-    <t>V59</t>
-  </si>
-  <si>
-    <t>V60</t>
-  </si>
-  <si>
-    <t>V61</t>
-  </si>
-  <si>
-    <t>V62</t>
-  </si>
-  <si>
-    <t>V63</t>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>alu</t>
+  </si>
+  <si>
+    <t>ctrl</t>
   </si>
 </sst>
 </file>
@@ -635,25 +538,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2829AC-3DF2-4F58-BBB1-B294A5BD73D1}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S87"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,337 +1357,367 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>7411</v>
-      </c>
-    </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>7410</v>
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>7410</v>
+        <v>7411</v>
+      </c>
+      <c r="C27">
+        <v>7430</v>
+      </c>
+      <c r="D27">
+        <v>7430</v>
+      </c>
+      <c r="E27">
+        <v>7408</v>
+      </c>
+      <c r="F27">
+        <v>7400</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>7404</v>
+        <v>7410</v>
+      </c>
+      <c r="C28">
+        <v>7411</v>
+      </c>
+      <c r="D28">
+        <v>7430</v>
+      </c>
+      <c r="E28">
+        <v>7400</v>
+      </c>
+      <c r="F28">
+        <v>7410</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>7410</v>
       </c>
+      <c r="C29">
+        <v>7410</v>
+      </c>
+      <c r="D29">
+        <v>7430</v>
+      </c>
+      <c r="E29">
+        <v>7400</v>
+      </c>
+      <c r="F29">
+        <v>7430</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>7404</v>
+      </c>
+      <c r="C30">
+        <v>7432</v>
+      </c>
+      <c r="D30">
+        <v>7400</v>
+      </c>
+      <c r="E30">
+        <v>7410</v>
+      </c>
+      <c r="F30">
+        <v>74245</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>7410</v>
+      </c>
+      <c r="C31">
+        <v>7404</v>
+      </c>
+      <c r="D31">
+        <v>7432</v>
+      </c>
+      <c r="E31">
+        <v>7400</v>
+      </c>
+      <c r="F31">
+        <v>74245</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>7408</v>
+      </c>
+      <c r="C32">
+        <v>7430</v>
+      </c>
+      <c r="D32">
+        <v>7408</v>
+      </c>
+      <c r="E32">
+        <v>7400</v>
+      </c>
+      <c r="F32">
+        <v>74245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>7430</v>
+      </c>
+      <c r="C33">
+        <v>7410</v>
+      </c>
+      <c r="D33">
+        <v>7432</v>
+      </c>
+      <c r="E33">
+        <v>7411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B34">
+        <v>7430</v>
+      </c>
+      <c r="C34">
+        <v>7400</v>
+      </c>
+      <c r="D34">
+        <v>7400</v>
+      </c>
+      <c r="E34">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35">
+        <v>7400</v>
+      </c>
+      <c r="C35">
+        <v>7400</v>
+      </c>
+      <c r="D35">
+        <v>7408</v>
+      </c>
+      <c r="E35">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B34">
+      <c r="B36">
+        <v>7432</v>
+      </c>
+      <c r="C36">
+        <v>7410</v>
+      </c>
+      <c r="D36">
+        <v>7410</v>
+      </c>
+      <c r="E36">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>7400</v>
+      </c>
+      <c r="C37">
+        <v>7432</v>
+      </c>
+      <c r="D37">
+        <v>7432</v>
+      </c>
+      <c r="E37">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38">
+        <v>7404</v>
+      </c>
+      <c r="E38">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39">
         <v>7408</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="E39">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="D40">
+        <v>7408</v>
+      </c>
+      <c r="E40">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="D41">
+        <v>7400</v>
+      </c>
+      <c r="E41">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D42">
+        <v>7432</v>
+      </c>
+      <c r="E42">
+        <v>7411</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D43">
+        <v>7432</v>
+      </c>
+      <c r="E43">
+        <v>7430</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="E44">
+        <v>7430</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="E45">
+        <v>7432</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="E46">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E47">
+        <v>7430</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="E48">
+        <v>7432</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="E49">
+        <v>7411</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="E50">
+        <v>7430</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="E51">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>89</v>
+      <c r="E52">
+        <v>7410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added last missing IC
</commit_message>
<xml_diff>
--- a/IC.xlsx
+++ b/IC.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\Desktop\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6917CC24-2E15-4533-9E32-9042E6AFD5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8509AEB1-AD7F-4C83-B127-B9BCD4372AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="1905" windowWidth="20070" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -261,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,7 +540,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1495,7 @@
         <v>74245</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1513,8 +1511,11 @@
       <c r="E33">
         <v>7411</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>7410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>7410</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>7410</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>7410</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>7410</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>7410</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>7411</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>7430</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>7430</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>7432</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>7430</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>

</xml_diff>